<commit_message>
feat: update preferences order evalution
</commit_message>
<xml_diff>
--- a/results/20250402/evaluation_GpositivePseAAC_noisy_0.0.xlsx
+++ b/results/20250402/evaluation_GpositivePseAAC_noisy_0.0.xlsx
@@ -1473,10 +1473,10 @@
         </is>
       </c>
       <c r="H26" t="n">
-        <v>0.2419</v>
+        <v>0.75718</v>
       </c>
       <c r="I26" t="n">
-        <v>0.04798</v>
+        <v>0.02112</v>
       </c>
     </row>
     <row r="27">
@@ -1512,10 +1512,10 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>0.10034</v>
+        <v>0.54134</v>
       </c>
       <c r="I27" t="n">
-        <v>0.04298</v>
+        <v>0.03794</v>
       </c>
     </row>
     <row r="28">
@@ -1553,10 +1553,10 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>0.24772</v>
+        <v>0.75621</v>
       </c>
       <c r="I28" t="n">
-        <v>0.05188</v>
+        <v>0.02167</v>
       </c>
     </row>
     <row r="29">
@@ -1594,10 +1594,10 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>0.10035</v>
+        <v>0.5394</v>
       </c>
       <c r="I29" t="n">
-        <v>0.04757</v>
+        <v>0.04133</v>
       </c>
     </row>
     <row r="30">
@@ -1633,10 +1633,10 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>0.24223</v>
+        <v>0.75782</v>
       </c>
       <c r="I30" t="n">
-        <v>0.04962</v>
+        <v>0.01999</v>
       </c>
     </row>
     <row r="31">
@@ -1672,10 +1672,10 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>0.1042</v>
+        <v>0.54326</v>
       </c>
       <c r="I31" t="n">
-        <v>0.04548</v>
+        <v>0.03847</v>
       </c>
     </row>
     <row r="32">
@@ -1713,10 +1713,10 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>0.24129</v>
+        <v>0.75686</v>
       </c>
       <c r="I32" t="n">
-        <v>0.05283</v>
+        <v>0.02081</v>
       </c>
     </row>
     <row r="33">
@@ -1754,10 +1754,10 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>0.10228</v>
+        <v>0.54711</v>
       </c>
       <c r="I33" t="n">
-        <v>0.04717</v>
+        <v>0.04153</v>
       </c>
     </row>
     <row r="34">
@@ -1793,10 +1793,10 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>0.25475</v>
+        <v>0.75526</v>
       </c>
       <c r="I34" t="n">
-        <v>0.04422</v>
+        <v>0.02279</v>
       </c>
     </row>
     <row r="35">
@@ -1832,10 +1832,10 @@
         </is>
       </c>
       <c r="H35" t="n">
-        <v>0.11189</v>
+        <v>0.52591</v>
       </c>
       <c r="I35" t="n">
-        <v>0.04078</v>
+        <v>0.04214</v>
       </c>
     </row>
     <row r="36">
@@ -1873,10 +1873,10 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>0.2493</v>
+        <v>0.75428</v>
       </c>
       <c r="I36" t="n">
-        <v>0.04541</v>
+        <v>0.02494</v>
       </c>
     </row>
     <row r="37">
@@ -1914,10 +1914,10 @@
         </is>
       </c>
       <c r="H37" t="n">
-        <v>0.10612</v>
+        <v>0.52976</v>
       </c>
       <c r="I37" t="n">
-        <v>0.04321</v>
+        <v>0.0456</v>
       </c>
     </row>
     <row r="38">
@@ -1953,10 +1953,10 @@
         </is>
       </c>
       <c r="H38" t="n">
-        <v>0.25862</v>
+        <v>0.75527</v>
       </c>
       <c r="I38" t="n">
-        <v>0.04442</v>
+        <v>0.02199</v>
       </c>
     </row>
     <row r="39">
@@ -1992,10 +1992,10 @@
         </is>
       </c>
       <c r="H39" t="n">
-        <v>0.11576</v>
+        <v>0.52399</v>
       </c>
       <c r="I39" t="n">
-        <v>0.04238</v>
+        <v>0.0413</v>
       </c>
     </row>
     <row r="40">
@@ -2033,10 +2033,10 @@
         </is>
       </c>
       <c r="H40" t="n">
-        <v>0.25124</v>
+        <v>0.75526</v>
       </c>
       <c r="I40" t="n">
-        <v>0.04779</v>
+        <v>0.02398</v>
       </c>
     </row>
     <row r="41">
@@ -2074,10 +2074,10 @@
         </is>
       </c>
       <c r="H41" t="n">
-        <v>0.10807</v>
+        <v>0.52976</v>
       </c>
       <c r="I41" t="n">
-        <v>0.04676</v>
+        <v>0.0456</v>
       </c>
     </row>
     <row r="42">
@@ -3073,10 +3073,10 @@
         </is>
       </c>
       <c r="H66" t="n">
-        <v>0.2024</v>
+        <v>0.75139</v>
       </c>
       <c r="I66" t="n">
-        <v>0.05251</v>
+        <v>0.03288</v>
       </c>
     </row>
     <row r="67">
@@ -3112,10 +3112,10 @@
         </is>
       </c>
       <c r="H67" t="n">
-        <v>0.0983</v>
+        <v>0.55674</v>
       </c>
       <c r="I67" t="n">
-        <v>0.04369</v>
+        <v>0.05356</v>
       </c>
     </row>
     <row r="68">
@@ -3153,10 +3153,10 @@
         </is>
       </c>
       <c r="H68" t="n">
-        <v>0.18732</v>
+        <v>0.75493</v>
       </c>
       <c r="I68" t="n">
-        <v>0.05185</v>
+        <v>0.02903</v>
       </c>
     </row>
     <row r="69">
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="H69" t="n">
-        <v>0.09249</v>
+        <v>0.58562</v>
       </c>
       <c r="I69" t="n">
-        <v>0.03924</v>
+        <v>0.05369</v>
       </c>
     </row>
     <row r="70">
@@ -3233,10 +3233,10 @@
         </is>
       </c>
       <c r="H70" t="n">
-        <v>0.20304</v>
+        <v>0.75235</v>
       </c>
       <c r="I70" t="n">
-        <v>0.05218</v>
+        <v>0.03285</v>
       </c>
     </row>
     <row r="71">
@@ -3272,10 +3272,10 @@
         </is>
       </c>
       <c r="H71" t="n">
-        <v>0.0983</v>
+        <v>0.55674</v>
       </c>
       <c r="I71" t="n">
-        <v>0.04369</v>
+        <v>0.05356</v>
       </c>
     </row>
     <row r="72">
@@ -3313,10 +3313,10 @@
         </is>
       </c>
       <c r="H72" t="n">
-        <v>0.19633</v>
+        <v>0.7517200000000001</v>
       </c>
       <c r="I72" t="n">
-        <v>0.05408</v>
+        <v>0.03037</v>
       </c>
     </row>
     <row r="73">
@@ -3354,10 +3354,10 @@
         </is>
       </c>
       <c r="H73" t="n">
-        <v>0.10213</v>
+        <v>0.57985</v>
       </c>
       <c r="I73" t="n">
-        <v>0.03877</v>
+        <v>0.0538</v>
       </c>
     </row>
     <row r="74">
@@ -3393,10 +3393,10 @@
         </is>
       </c>
       <c r="H74" t="n">
-        <v>0.21072</v>
+        <v>0.75236</v>
       </c>
       <c r="I74" t="n">
-        <v>0.04957</v>
+        <v>0.02674</v>
       </c>
     </row>
     <row r="75">
@@ -3432,10 +3432,10 @@
         </is>
       </c>
       <c r="H75" t="n">
-        <v>0.11561</v>
+        <v>0.55097</v>
       </c>
       <c r="I75" t="n">
-        <v>0.0408</v>
+        <v>0.05156</v>
       </c>
     </row>
     <row r="76">
@@ -3473,10 +3473,10 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>0.20015</v>
+        <v>0.75396</v>
       </c>
       <c r="I76" t="n">
-        <v>0.05367</v>
+        <v>0.02799</v>
       </c>
     </row>
     <row r="77">
@@ -3514,10 +3514,10 @@
         </is>
       </c>
       <c r="H77" t="n">
-        <v>0.1098</v>
+        <v>0.57212</v>
       </c>
       <c r="I77" t="n">
-        <v>0.0432</v>
+        <v>0.06347999999999999</v>
       </c>
     </row>
     <row r="78">
@@ -3553,10 +3553,10 @@
         </is>
       </c>
       <c r="H78" t="n">
-        <v>0.21072</v>
+        <v>0.75236</v>
       </c>
       <c r="I78" t="n">
-        <v>0.04957</v>
+        <v>0.02674</v>
       </c>
     </row>
     <row r="79">
@@ -3592,10 +3592,10 @@
         </is>
       </c>
       <c r="H79" t="n">
-        <v>0.11561</v>
+        <v>0.55097</v>
       </c>
       <c r="I79" t="n">
-        <v>0.0408</v>
+        <v>0.05156</v>
       </c>
     </row>
     <row r="80">
@@ -3633,10 +3633,10 @@
         </is>
       </c>
       <c r="H80" t="n">
-        <v>0.20015</v>
+        <v>0.75396</v>
       </c>
       <c r="I80" t="n">
-        <v>0.05367</v>
+        <v>0.02799</v>
       </c>
     </row>
     <row r="81">
@@ -3674,10 +3674,10 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>0.1098</v>
+        <v>0.57212</v>
       </c>
       <c r="I81" t="n">
-        <v>0.0432</v>
+        <v>0.06347999999999999</v>
       </c>
     </row>
     <row r="82">
@@ -4673,10 +4673,10 @@
         </is>
       </c>
       <c r="H106" t="n">
-        <v>0.25733</v>
+        <v>0.75012</v>
       </c>
       <c r="I106" t="n">
-        <v>0.04509</v>
+        <v>0.02101</v>
       </c>
     </row>
     <row r="107">
@@ -4712,10 +4712,10 @@
         </is>
       </c>
       <c r="H107" t="n">
-        <v>0.11372</v>
+        <v>0.51819</v>
       </c>
       <c r="I107" t="n">
-        <v>0.01575</v>
+        <v>0.04992</v>
       </c>
     </row>
     <row r="108">
@@ -4753,10 +4753,10 @@
         </is>
       </c>
       <c r="H108" t="n">
-        <v>0.26342</v>
+        <v>0.74947</v>
       </c>
       <c r="I108" t="n">
-        <v>0.04124</v>
+        <v>0.01935</v>
       </c>
     </row>
     <row r="109">
@@ -4794,10 +4794,10 @@
         </is>
       </c>
       <c r="H109" t="n">
-        <v>0.11755</v>
+        <v>0.51434</v>
       </c>
       <c r="I109" t="n">
-        <v>0.01291</v>
+        <v>0.04622</v>
       </c>
     </row>
     <row r="110">
@@ -4833,10 +4833,10 @@
         </is>
       </c>
       <c r="H110" t="n">
-        <v>0.25989</v>
+        <v>0.75076</v>
       </c>
       <c r="I110" t="n">
-        <v>0.04589</v>
+        <v>0.02126</v>
       </c>
     </row>
     <row r="111">
@@ -4872,10 +4872,10 @@
         </is>
       </c>
       <c r="H111" t="n">
-        <v>0.11757</v>
+        <v>0.51819</v>
       </c>
       <c r="I111" t="n">
-        <v>0.01789</v>
+        <v>0.04992</v>
       </c>
     </row>
     <row r="112">
@@ -4913,10 +4913,10 @@
         </is>
       </c>
       <c r="H112" t="n">
-        <v>0.26244</v>
+        <v>0.75204</v>
       </c>
       <c r="I112" t="n">
-        <v>0.04017</v>
+        <v>0.02031</v>
       </c>
     </row>
     <row r="113">
@@ -4954,10 +4954,10 @@
         </is>
       </c>
       <c r="H113" t="n">
-        <v>0.1214</v>
+        <v>0.52013</v>
       </c>
       <c r="I113" t="n">
-        <v>0.01312</v>
+        <v>0.04398</v>
       </c>
     </row>
     <row r="114">
@@ -4993,10 +4993,10 @@
         </is>
       </c>
       <c r="H114" t="n">
-        <v>0.25927</v>
+        <v>0.74626</v>
       </c>
       <c r="I114" t="n">
-        <v>0.0379</v>
+        <v>0.01848</v>
       </c>
     </row>
     <row r="115">
@@ -5032,10 +5032,10 @@
         </is>
       </c>
       <c r="H115" t="n">
-        <v>0.10218</v>
+        <v>0.5123799999999999</v>
       </c>
       <c r="I115" t="n">
-        <v>0.01831</v>
+        <v>0.05367</v>
       </c>
     </row>
     <row r="116">
@@ -5073,10 +5073,10 @@
         </is>
       </c>
       <c r="H116" t="n">
-        <v>0.25767</v>
+        <v>0.74819</v>
       </c>
       <c r="I116" t="n">
-        <v>0.04202</v>
+        <v>0.01844</v>
       </c>
     </row>
     <row r="117">
@@ -5114,10 +5114,10 @@
         </is>
       </c>
       <c r="H117" t="n">
-        <v>0.09836</v>
+        <v>0.5143</v>
       </c>
       <c r="I117" t="n">
-        <v>0.02364</v>
+        <v>0.05196</v>
       </c>
     </row>
     <row r="118">
@@ -5153,10 +5153,10 @@
         </is>
       </c>
       <c r="H118" t="n">
-        <v>0.25927</v>
+        <v>0.74626</v>
       </c>
       <c r="I118" t="n">
-        <v>0.0379</v>
+        <v>0.01848</v>
       </c>
     </row>
     <row r="119">
@@ -5192,10 +5192,10 @@
         </is>
       </c>
       <c r="H119" t="n">
-        <v>0.10218</v>
+        <v>0.5123799999999999</v>
       </c>
       <c r="I119" t="n">
-        <v>0.01831</v>
+        <v>0.05367</v>
       </c>
     </row>
     <row r="120">
@@ -5233,10 +5233,10 @@
         </is>
       </c>
       <c r="H120" t="n">
-        <v>0.25767</v>
+        <v>0.74819</v>
       </c>
       <c r="I120" t="n">
-        <v>0.04202</v>
+        <v>0.01844</v>
       </c>
     </row>
     <row r="121">
@@ -5274,10 +5274,10 @@
         </is>
       </c>
       <c r="H121" t="n">
-        <v>0.09836</v>
+        <v>0.5143</v>
       </c>
       <c r="I121" t="n">
-        <v>0.02364</v>
+        <v>0.05196</v>
       </c>
     </row>
     <row r="122">
@@ -6273,10 +6273,10 @@
         </is>
       </c>
       <c r="H146" t="n">
-        <v>0.18793</v>
+        <v>0.76744</v>
       </c>
       <c r="I146" t="n">
-        <v>0.04265</v>
+        <v>0.02874</v>
       </c>
     </row>
     <row r="147">
@@ -6312,10 +6312,10 @@
         </is>
       </c>
       <c r="H147" t="n">
-        <v>0.09059</v>
+        <v>0.59139</v>
       </c>
       <c r="I147" t="n">
-        <v>0.02338</v>
+        <v>0.05296</v>
       </c>
     </row>
     <row r="148">
@@ -6353,10 +6353,10 @@
         </is>
       </c>
       <c r="H148" t="n">
-        <v>0.18181</v>
+        <v>0.76871</v>
       </c>
       <c r="I148" t="n">
-        <v>0.03986</v>
+        <v>0.03012</v>
       </c>
     </row>
     <row r="149">
@@ -6394,10 +6394,10 @@
         </is>
       </c>
       <c r="H149" t="n">
-        <v>0.08867</v>
+        <v>0.60103</v>
       </c>
       <c r="I149" t="n">
-        <v>0.02623</v>
+        <v>0.05116</v>
       </c>
     </row>
     <row r="150">
@@ -6433,10 +6433,10 @@
         </is>
       </c>
       <c r="H150" t="n">
-        <v>0.18889</v>
+        <v>0.76744</v>
       </c>
       <c r="I150" t="n">
-        <v>0.04413</v>
+        <v>0.02874</v>
       </c>
     </row>
     <row r="151">
@@ -6472,10 +6472,10 @@
         </is>
       </c>
       <c r="H151" t="n">
-        <v>0.09251</v>
+        <v>0.59139</v>
       </c>
       <c r="I151" t="n">
-        <v>0.02634</v>
+        <v>0.05296</v>
       </c>
     </row>
     <row r="152">
@@ -6513,10 +6513,10 @@
         </is>
       </c>
       <c r="H152" t="n">
-        <v>0.18116</v>
+        <v>0.77032</v>
       </c>
       <c r="I152" t="n">
-        <v>0.04041</v>
+        <v>0.03024</v>
       </c>
     </row>
     <row r="153">
@@ -6554,10 +6554,10 @@
         </is>
       </c>
       <c r="H153" t="n">
-        <v>0.09059</v>
+        <v>0.60487</v>
       </c>
       <c r="I153" t="n">
-        <v>0.02902</v>
+        <v>0.05208</v>
       </c>
     </row>
     <row r="154">
@@ -6593,10 +6593,10 @@
         </is>
       </c>
       <c r="H154" t="n">
-        <v>0.18953</v>
+        <v>0.76807</v>
       </c>
       <c r="I154" t="n">
-        <v>0.04436</v>
+        <v>0.02924</v>
       </c>
     </row>
     <row r="155">
@@ -6632,10 +6632,10 @@
         </is>
       </c>
       <c r="H155" t="n">
-        <v>0.08869</v>
+        <v>0.58178</v>
       </c>
       <c r="I155" t="n">
-        <v>0.02701</v>
+        <v>0.0484</v>
       </c>
     </row>
     <row r="156">
@@ -6673,10 +6673,10 @@
         </is>
       </c>
       <c r="H156" t="n">
-        <v>0.17732</v>
+        <v>0.76774</v>
       </c>
       <c r="I156" t="n">
-        <v>0.03835</v>
+        <v>0.02928</v>
       </c>
     </row>
     <row r="157">
@@ -6714,10 +6714,10 @@
         </is>
       </c>
       <c r="H157" t="n">
-        <v>0.08676</v>
+        <v>0.59718</v>
       </c>
       <c r="I157" t="n">
-        <v>0.02939</v>
+        <v>0.05065</v>
       </c>
     </row>
     <row r="158">
@@ -6753,10 +6753,10 @@
         </is>
       </c>
       <c r="H158" t="n">
-        <v>0.18953</v>
+        <v>0.76807</v>
       </c>
       <c r="I158" t="n">
-        <v>0.04436</v>
+        <v>0.02924</v>
       </c>
     </row>
     <row r="159">
@@ -6792,10 +6792,10 @@
         </is>
       </c>
       <c r="H159" t="n">
-        <v>0.08869</v>
+        <v>0.58178</v>
       </c>
       <c r="I159" t="n">
-        <v>0.02701</v>
+        <v>0.0484</v>
       </c>
     </row>
     <row r="160">
@@ -6833,10 +6833,10 @@
         </is>
       </c>
       <c r="H160" t="n">
-        <v>0.17539</v>
+        <v>0.76967</v>
       </c>
       <c r="I160" t="n">
-        <v>0.03677</v>
+        <v>0.02766</v>
       </c>
     </row>
     <row r="161">
@@ -6874,10 +6874,10 @@
         </is>
       </c>
       <c r="H161" t="n">
-        <v>0.08676</v>
+        <v>0.60103</v>
       </c>
       <c r="I161" t="n">
-        <v>0.02939</v>
+        <v>0.05116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>